<commit_message>
enable CIs to have differing confidence levels, not just 95%
</commit_message>
<xml_diff>
--- a/rgStandardized_worksheet.xlsx
+++ b/rgStandardized_worksheet.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,9 +9,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelrosin/Dropbox/_UNC/_Draft_Paper1/rgStandardized/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B5F05D6-CD51-8746-B375-501C0C8B22F2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D6CAFDE-789A-B84D-ACDA-8D08CF530869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{9FB095F8-04E3-A34D-8D2C-66F28D0EA142}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{9FB095F8-04E3-A34D-8D2C-66F28D0EA142}"/>
   </bookViews>
   <sheets>
     <sheet name="standardized Rogan-Gladen" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="24">
   <si>
     <t>Stratum</t>
   </si>
@@ -57,12 +57,6 @@
   </si>
   <si>
     <t>Point estimate</t>
-  </si>
-  <si>
-    <t>95% CI, lower bound</t>
-  </si>
-  <si>
-    <t>95% CI, upper bound</t>
   </si>
   <si>
     <t>Sensitivity estimate</t>
@@ -107,13 +101,22 @@
     <t>Instructions: Data are entered in the orange input cells and the main results are given at the table at the top-right. Intermediate results are in the grey calculation cells and, except for the estimates of sensitivity and specificity, should not be reported.</t>
   </si>
   <si>
-    <t xml:space="preserve">Written to accompany the manuscript “Estimating Seroprevalence of SARS-CoV-2”. These spreadsheets may be shared freely. No warranty is implied about the accuracy of the results. Correspondence to srosin@live.unc.edu.   </t>
+    <t>Alpha level (1 - confidence level)</t>
+  </si>
+  <si>
+    <t>CI, lower bound</t>
+  </si>
+  <si>
+    <t>CI, upper bound</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -269,7 +272,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -288,8 +291,6 @@
     <xf numFmtId="10" fontId="3" fillId="3" borderId="5" xfId="3" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="3" fillId="3" borderId="6" xfId="3" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="3" fillId="3" borderId="7" xfId="3" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="3" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -297,6 +298,7 @@
     <xf numFmtId="1" fontId="3" fillId="3" borderId="4" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="6" xfId="3" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -859,7 +861,7 @@
   <dimension ref="A1:I95"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -868,148 +870,152 @@
     <col min="3" max="3" width="20" customWidth="1"/>
     <col min="4" max="4" width="21.33203125" customWidth="1"/>
     <col min="5" max="5" width="25.5" customWidth="1"/>
-    <col min="6" max="6" width="19.83203125" customWidth="1"/>
+    <col min="6" max="6" width="26.83203125" customWidth="1"/>
     <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.83203125" customWidth="1"/>
     <col min="9" max="9" width="22.6640625" customWidth="1"/>
     <col min="10" max="10" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
       <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="F2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="11" t="str">
-        <f>IF(H12="","",(H15+H12-1)/(C12+H12-1))</f>
-        <v/>
+    <row r="2" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="8">
+        <v>0.05</v>
       </c>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="F3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="20" t="str">
-        <f>IF(F16="","",(D12+I12+SUM(F16:F95))/(C12+H12-1)^2)</f>
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="F3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="11" t="str">
+        <f>IF(H12="","",(H15+H12-1)/(C12+H12-1))</f>
         <v/>
       </c>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="F4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="12" t="str">
-        <f>IF(G3="","",G2-NORMSINV(0.975)*SQRT(G3))</f>
+      <c r="F4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="18" t="str">
+        <f>IF(F16="","",(D12+I12+SUM(F16:F95))/(C12+H12-1)^2)</f>
         <v/>
       </c>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="F5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="F5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="13" t="str">
-        <f>IF(G3="","",G2+NORMSINV(0.975)*SQRT(G3))</f>
+      <c r="G5" s="12" t="str">
+        <f>IF(G4="","",G3-NORMSINV(1-$G$2/2)*SQRT(G4))</f>
         <v/>
       </c>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="15"/>
+    <row r="6" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="21"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="F6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="13" t="str">
+        <f>IF(G4="","",G3+NORMSINV(1-$G$2/2)*SQRT(G4))</f>
+        <v/>
+      </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="22"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="22"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
+      <c r="A9" s="14"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="F10" s="21" t="s">
+      <c r="B10" s="20"/>
+      <c r="F10" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="G10" s="21"/>
+      <c r="G10" s="20"/>
     </row>
     <row r="11" spans="1:9" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" t="s">
         <v>17</v>
       </c>
-      <c r="B11" t="s">
+      <c r="H11" t="s">
         <v>18</v>
       </c>
-      <c r="C11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" t="s">
-        <v>20</v>
-      </c>
       <c r="I11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -1019,8 +1025,8 @@
         <f>IF(A12="","",B12/A12)</f>
         <v/>
       </c>
-      <c r="D12" s="17" t="str">
-        <f>IF(A12="","",G2^2*C12*(1-C12)/A12)</f>
+      <c r="D12" s="15" t="str">
+        <f>IF(A12="","",G3^2*C12*(1-C12)/A12)</f>
         <v/>
       </c>
       <c r="F12" s="8"/>
@@ -1029,38 +1035,38 @@
         <f>IF(F12="","",1-(G12/F12))</f>
         <v/>
       </c>
-      <c r="I12" s="19" t="str">
-        <f>IF(F12="","",(1-G2)^2*H12*(1-H12)/F12)</f>
+      <c r="I12" s="17" t="str">
+        <f>IF(F12="","",(1-G3)^2*H12*(1-H12)/F12)</f>
         <v/>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="21"/>
+      <c r="B14" s="20"/>
     </row>
     <row r="15" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="E15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="F15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="7" t="s">
         <v>13</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>15</v>
       </c>
       <c r="H15" s="9" t="str">
         <f>IF(E16="","",SUMPRODUCT(B16:B95,E16:E95))</f>
@@ -2445,7 +2451,7 @@
   <dimension ref="A1:I95"/>
   <sheetViews>
     <sheetView zoomScale="145" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2461,141 +2467,145 @@
     <col min="10" max="10" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
       <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="F2" s="1" t="s">
+    <row r="2" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="F3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="11">
+      <c r="G3" s="11">
         <f>IF(H12="","",(H15+H12-1)/(C12+H12-1))</f>
         <v>0.31457664233576638</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="F3" s="2" t="s">
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="20">
+      <c r="G4" s="19">
         <f>IF(F16="","",(D12+I12+SUM(F16:F95))/(C12+H12-1)^2)</f>
         <v>2.228294749180685E-3</v>
       </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="F4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="12">
-        <f>IF(G3="","",G2-NORMSINV(0.975)*SQRT(G3))</f>
-        <v>0.22205690109452347</v>
-      </c>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="F5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="F5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="13">
-        <f>IF(G3="","",G2+NORMSINV(0.975)*SQRT(G3))</f>
-        <v>0.40709638357700928</v>
+      <c r="G5" s="12">
+        <f>IF(G4="","",G3-NORMSINV(1-$G$2/2)*SQRT(G4))</f>
+        <v>0.22205690109452347</v>
       </c>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="15"/>
+    <row r="6" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="21"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="F6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="13">
+        <f>IF(G4="","",G3+NORMSINV(1-$G$2/2)*SQRT(G4))</f>
+        <v>0.40709638357700928</v>
+      </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="22"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="22"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
+      <c r="A9" s="14"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="F10" s="21" t="s">
+      <c r="B10" s="20"/>
+      <c r="F10" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="G10" s="21"/>
+      <c r="G10" s="20"/>
     </row>
     <row r="11" spans="1:9" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" t="s">
         <v>17</v>
       </c>
-      <c r="B11" t="s">
+      <c r="H11" t="s">
         <v>18</v>
       </c>
-      <c r="C11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" t="s">
-        <v>20</v>
-      </c>
       <c r="I11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -2609,8 +2619,8 @@
         <f>IF(A12="","",B12/A12)</f>
         <v>1</v>
       </c>
-      <c r="D12" s="18">
-        <f>IF(A12="","",G2^2*C12*(1-C12)/A12)</f>
+      <c r="D12" s="16">
+        <f>IF(A12="","",G3^2*C12*(1-C12)/A12)</f>
         <v>0</v>
       </c>
       <c r="F12" s="8">
@@ -2623,38 +2633,38 @@
         <f>IF(F12="","",1-(G12/F12))</f>
         <v>0.98916967509025266</v>
       </c>
-      <c r="I12" s="19">
-        <f>IF(F12="","",(1-G2)^2*H12*(1-H12)/F12)</f>
+      <c r="I12" s="17">
+        <f>IF(F12="","",(1-G3)^2*H12*(1-H12)/F12)</f>
         <v>1.8169806846030277E-5</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="21"/>
+      <c r="B14" s="20"/>
     </row>
     <row r="15" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="E15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="F15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="7" t="s">
         <v>13</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>15</v>
       </c>
       <c r="H15" s="9">
         <f>IF(E16="","",SUMPRODUCT(B16:B95,E16:E95))</f>

</xml_diff>